<commit_message>
add windows login; init Users maintain page;
</commit_message>
<xml_diff>
--- a/Template MVC.xlsx
+++ b/Template MVC.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\DF\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program\WebTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2205" windowHeight="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Account" sheetId="2" r:id="rId1"/>
+    <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="INI" sheetId="6" r:id="rId2"/>
     <sheet name="Transaction_Log" sheetId="5" r:id="rId3"/>
     <sheet name="Role" sheetId="3" r:id="rId4"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="64">
   <si>
     <t>Table Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,10 +98,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Acc_No</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Active</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -118,10 +114,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Account</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Role</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -138,42 +130,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LastLogin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DATETIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Psw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VARCHAR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Acc_Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VARCHAR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Setting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Application_Name</t>
   </si>
   <si>
@@ -246,6 +210,65 @@
   </si>
   <si>
     <t>''</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>userno</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_admin</t>
+  </si>
+  <si>
+    <t>lastlogin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cdt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATETIME2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATETIME2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Users</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -613,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H15"/>
+      <selection activeCell="H6" sqref="H6:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -636,18 +659,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G2" t="str">
         <f>"IF  EXISTS (SELECT * FROM sys.objects WHERE object_id = OBJECT_ID(N'[dbo].["&amp;$B$1&amp;"]') AND type in (N'U')) DROP TABLE [dbo].["&amp;$B$1&amp;"] "</f>
-        <v xml:space="preserve">IF  EXISTS (SELECT * FROM sys.objects WHERE object_id = OBJECT_ID(N'[dbo].[Account]') AND type in (N'U')) DROP TABLE [dbo].[Account] </v>
+        <v xml:space="preserve">IF  EXISTS (SELECT * FROM sys.objects WHERE object_id = OBJECT_ID(N'[dbo].[Users]') AND type in (N'U')) DROP TABLE [dbo].[Users] </v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -668,7 +691,7 @@
       </c>
       <c r="G4" t="str">
         <f>"CREATE TABLE "&amp;B1&amp;"("</f>
-        <v>CREATE TABLE Account(</v>
+        <v>CREATE TABLE Users(</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -676,21 +699,18 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="G5" t="str">
-        <f>B5&amp;" "&amp;C5&amp;IF(E5=1,""," NOT NULL ")&amp;IF(D5&lt;&gt;"","("&amp;D5&amp;"),",",")</f>
-        <v>Id UNIQUEIDENTIFIER NOT NULL ,</v>
+        <f>B5&amp;" "&amp;C5&amp;" IDENTITY, "</f>
+        <v xml:space="preserve">user_id INT IDENTITY, </v>
       </c>
       <c r="H5" t="str">
         <f>"ALTER TABLE " &amp; $B$1 &amp;" ADD CONSTRAINT df_" &amp; $B$1 &amp;"_"&amp; B5&amp; " DEFAULT "&amp;F5&amp;" FOR " &amp; B5</f>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Id DEFAULT NEWID() FOR Id</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_user_id DEFAULT  FOR user_id</v>
       </c>
       <c r="N5" t="s">
         <v>7</v>
@@ -698,29 +718,29 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G6" t="str">
         <f>B6 &amp; " " &amp; C6 &amp; IF(D6&lt;&gt;"","("&amp;D6&amp;")","") &amp; IF(E6=1,","," NOT NULL ,")</f>
-        <v>Acc_Name NVARCHAR(20) NOT NULL ,</v>
+        <v>username NVARCHAR(50) NOT NULL ,</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" ref="H6:H15" si="0">"ALTER TABLE " &amp; $B$1 &amp;" ADD CONSTRAINT df_" &amp; $B$1 &amp;"_"&amp; B6&amp; " DEFAULT "&amp;F6&amp;" FOR " &amp; B6</f>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Acc_Name DEFAULT '' FOR Acc_Name</v>
+        <f t="shared" ref="H6:H16" si="0">"ALTER TABLE " &amp; $B$1 &amp;" ADD CONSTRAINT df_" &amp; $B$1 &amp;"_"&amp; B6&amp; " DEFAULT "&amp;F6&amp;" FOR " &amp; B6</f>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_username DEFAULT '' FOR username</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -729,189 +749,208 @@
         <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" ref="G7:G15" si="1">B7 &amp; " " &amp; C7 &amp; IF(D7&lt;&gt;"","("&amp;D7&amp;")","") &amp; IF(E7=1,","," NOT NULL ,")</f>
-        <v>Acc_No VARCHAR(20) NOT NULL ,</v>
+        <f t="shared" ref="G7:G16" si="1">B7 &amp; " " &amp; C7 &amp; IF(D7&lt;&gt;"","("&amp;D7&amp;")","") &amp; IF(E7=1,","," NOT NULL ,")</f>
+        <v>userno VARCHAR(20) NOT NULL ,</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Acc_No DEFAULT '' FOR Acc_No</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_userno DEFAULT '' FOR userno</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D8">
-        <v>200</v>
+        <v>255</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>Psw VARCHAR(200) NOT NULL ,</v>
+        <v>password VARCHAR(255) NOT NULL ,</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Psw DEFAULT '' FOR Psw</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_password DEFAULT '' FOR password</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>Active BIT NOT NULL ,</v>
+        <v>is_active BIT NOT NULL ,</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Active DEFAULT 0 FOR Active</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_is_active DEFAULT 0 FOR is_active</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10">
-        <v>200</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="1"/>
-        <v>Email VARCHAR(200) NOT NULL ,</v>
+        <f t="shared" ref="G10" si="2">B10 &amp; " " &amp; C10 &amp; IF(D10&lt;&gt;"","("&amp;D10&amp;")","") &amp; IF(E10=1,","," NOT NULL ,")</f>
+        <v>is_admin BIT NOT NULL ,</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Email DEFAULT '' FOR Email</v>
+        <f t="shared" ref="H10" si="3">"ALTER TABLE " &amp; $B$1 &amp;" ADD CONSTRAINT df_" &amp; $B$1 &amp;"_"&amp; B10&amp; " DEFAULT "&amp;F10&amp;" FOR " &amp; B10</f>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_is_admin DEFAULT 0 FOR is_admin</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G11" t="str">
-        <f>B11 &amp; " " &amp; C11 &amp; IF(D11&lt;&gt;"","("&amp;D11&amp;")","") &amp; IF(E11=1,","," NOT NULL ,")</f>
-        <v>Role VARCHAR(3) NOT NULL ,</v>
+        <f t="shared" si="1"/>
+        <v>email VARCHAR(200) NOT NULL ,</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Role DEFAULT '' FOR Role</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_email DEFAULT '' FOR email</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="1"/>
-        <v>LastLogin DATETIME,</v>
+        <f>B12 &amp; " " &amp; C12 &amp; IF(D12&lt;&gt;"","("&amp;D12&amp;")","") &amp; IF(E12=1,","," NOT NULL ,")</f>
+        <v>role VARCHAR(10) NOT NULL ,</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_LastLogin DEFAULT GETDATE() FOR LastLogin</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_role DEFAULT '' FOR role</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13">
-        <v>1000</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
-        <v>Setting VARCHAR(1000) NOT NULL ,</v>
+        <v>lastlogin DATETIME2,</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Setting DEFAULT '' FOR Setting</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_lastlogin DEFAULT GETDATE() FOR lastlogin</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
-        <v>Remark VARCHAR(200) NOT NULL ,</v>
+        <v>setting VARCHAR(1000) NOT NULL ,</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Remark DEFAULT '' FOR Remark</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_setting DEFAULT '' FOR setting</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>200</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>remark VARCHAR(200) NOT NULL ,</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_remark DEFAULT '' FOR remark</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
         <v>16</v>
       </c>
-      <c r="G15" t="str">
-        <f t="shared" si="1"/>
-        <v>Cdt DATETIME NOT NULL ,</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v>ALTER TABLE Account ADD CONSTRAINT df_Account_Cdt DEFAULT GETDATE() FOR Cdt</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G16" t="s">
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>cdt DATETIME2 NOT NULL ,</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_cdt DEFAULT GETDATE() FOR cdt</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -924,10 +963,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -947,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -958,7 +997,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -985,7 +1024,7 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1013,7 +1052,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1022,7 +1061,7 @@
         <v>100</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G6" t="str">
         <f>B6 &amp; " " &amp; C6 &amp; IF(D6&lt;&gt;"","("&amp;D6&amp;")","") &amp; IF(E6=1,","," NOT NULL ,")</f>
@@ -1039,7 +1078,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -1048,7 +1087,7 @@
         <v>4000</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ref="G7:G11" si="2">B7 &amp; " " &amp; C7 &amp; IF(D7&lt;&gt;"","("&amp;D7&amp;")","") &amp; IF(E7=1,","," NOT NULL ,")</f>
@@ -1065,7 +1104,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -1074,7 +1113,7 @@
         <v>1000</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="2"/>
@@ -1091,7 +1130,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -1100,7 +1139,7 @@
         <v>100</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="2"/>
@@ -1140,7 +1179,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1164,6 +1203,29 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="str">
+        <f>B17&amp;" "&amp;C17&amp;IF(E17=1,""," NOT NULL ")&amp;IF(D17&lt;&gt;"","("&amp;D17&amp;"),",",")</f>
+        <v>Id UNIQUEIDENTIFIER NOT NULL ,</v>
+      </c>
+      <c r="H17" t="str">
+        <f>"ALTER TABLE " &amp; $B$1 &amp;" ADD CONSTRAINT df_" &amp; $B$1 &amp;"_"&amp; B17&amp; " DEFAULT "&amp;F17&amp;" FOR " &amp; B17</f>
+        <v>ALTER TABLE INI ADD CONSTRAINT df_INI_Id DEFAULT NEWID() FOR Id</v>
+      </c>
+      <c r="I17" t="str">
+        <f>" ALTER TABLE "&amp;$B$1&amp;" DROP CONSTRAINT df_" &amp; $B$1 &amp;"_"&amp; B17</f>
+        <v xml:space="preserve"> ALTER TABLE INI DROP CONSTRAINT df_INI_Id</v>
       </c>
     </row>
   </sheetData>
@@ -1178,7 +1240,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1048576"/>
+      <selection activeCell="H5" sqref="H5:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1190,6 +1252,7 @@
     <col min="5" max="5" width="9.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.75" customWidth="1"/>
     <col min="10" max="10" width="76" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1198,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1209,7 +1272,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1236,7 +1299,7 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1267,10 +1330,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -1290,7 +1353,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1313,7 +1376,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1336,7 +1399,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -1359,7 +1422,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1436,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1487,10 +1550,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
       </c>
       <c r="G4" t="str">
         <f>B4 &amp; " " &amp; C4 &amp; IF(D4&lt;&gt;"","("&amp;D4&amp;")","") &amp; IF(E4=1,","," NOT NULL IDENTITY(1,1) ,")</f>
@@ -1503,7 +1566,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -1522,10 +1585,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
@@ -1538,10 +1601,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
       </c>
       <c r="D7">
         <v>3</v>

</xml_diff>

<commit_message>
finish admin/user/maintain edit, delete function; next: add user
</commit_message>
<xml_diff>
--- a/Template MVC.xlsx
+++ b/Template MVC.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
   <si>
     <t>Table Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -269,6 +269,18 @@
   </si>
   <si>
     <t>Users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'{}'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Member'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'example@email.com'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -639,7 +651,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:H16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -831,7 +843,7 @@
         <v>200</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -839,7 +851,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_email DEFAULT '' FOR email</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_email DEFAULT 'example@email.com' FOR email</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -853,7 +865,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="G12" t="str">
         <f>B12 &amp; " " &amp; C12 &amp; IF(D12&lt;&gt;"","("&amp;D12&amp;")","") &amp; IF(E12=1,","," NOT NULL ,")</f>
@@ -861,7 +873,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_role DEFAULT '' FOR role</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_role DEFAULT 'Member' FOR role</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -897,7 +909,7 @@
         <v>1000</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -905,7 +917,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_setting DEFAULT '' FOR setting</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_setting DEFAULT '{}' FOR setting</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -919,7 +931,7 @@
         <v>200</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -927,7 +939,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_remark DEFAULT '' FOR remark</v>
+        <v>ALTER TABLE Users ADD CONSTRAINT df_Users_remark DEFAULT '{}' FOR remark</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>